<commit_message>
add different refueling strategy
</commit_message>
<xml_diff>
--- a/Data_analysis.xlsx
+++ b/Data_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keran\Google Drive\MIT\Courses@MIT\Thesis\simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D960C423-9E8B-4BF4-AFE9-5549C86C91A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEC0A78-DC6B-4BD8-B14D-EAEF94EA808C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15900" yWindow="7485" windowWidth="7740" windowHeight="3060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ship" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
update on take-off simulation
</commit_message>
<xml_diff>
--- a/Data_analysis.xlsx
+++ b/Data_analysis.xlsx
@@ -8,36 +8,211 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keran\Google Drive\MIT\Courses@MIT\Thesis\simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEC0A78-DC6B-4BD8-B14D-EAEF94EA808C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F392F66B-5619-46CC-A9BB-D8F983139DC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15900" yWindow="7485" windowWidth="7740" windowHeight="3060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ship" sheetId="1" r:id="rId1"/>
+    <sheet name="Aircraft_main_affect" sheetId="2" r:id="rId2"/>
+    <sheet name="Refueling_aircraft" sheetId="3" r:id="rId3"/>
+    <sheet name="maxCl_aspect_ratio" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Aircraft_main_affect!$R$8:$R$15</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Aircraft_main_affect!$U$7</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Aircraft_main_affect!$U$8:$U$15</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Aircraft_main_affect!$U$8:$U$15</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Aircraft_main_affect!$R$8:$R$15</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Aircraft_main_affect!$U$8:$U$15</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>ship length</t>
   </si>
   <si>
     <t>multiplier</t>
   </si>
+  <si>
+    <t>wing_span</t>
+  </si>
+  <si>
+    <t>thr_w_ratio</t>
+  </si>
+  <si>
+    <t>aspect_ratio</t>
+  </si>
+  <si>
+    <t>sweep_angle</t>
+  </si>
+  <si>
+    <t>mto_weight</t>
+  </si>
+  <si>
+    <t>Takeoff distance</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Fuel_Consumed</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>500m</t>
+  </si>
+  <si>
+    <t>Wing span</t>
+  </si>
+  <si>
+    <t>Thr weight ratio</t>
+  </si>
+  <si>
+    <t>aspect ratio</t>
+  </si>
+  <si>
+    <t>sweep angle</t>
+  </si>
+  <si>
+    <t>max take-off weight</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>fuel cost</t>
+  </si>
+  <si>
+    <t>Delta W</t>
+  </si>
+  <si>
+    <t>707-320</t>
+  </si>
+  <si>
+    <t>E-6A</t>
+  </si>
+  <si>
+    <t>727-200</t>
+  </si>
+  <si>
+    <t>737-200</t>
+  </si>
+  <si>
+    <t>747-400</t>
+  </si>
+  <si>
+    <t>757-200</t>
+  </si>
+  <si>
+    <t>767-200</t>
+  </si>
+  <si>
+    <t>777-200</t>
+  </si>
+  <si>
+    <t>A321-200</t>
+  </si>
+  <si>
+    <t>L-1011</t>
+  </si>
+  <si>
+    <t>S-3A</t>
+  </si>
+  <si>
+    <t>DC-9</t>
+  </si>
+  <si>
+    <t>C-5A</t>
+  </si>
+  <si>
+    <t>F-16C</t>
+  </si>
+  <si>
+    <t>F-22A</t>
+  </si>
+  <si>
+    <t>A-3D</t>
+  </si>
+  <si>
+    <t>F-4B</t>
+  </si>
+  <si>
+    <t>A-4E</t>
+  </si>
+  <si>
+    <t>RA-5C</t>
+  </si>
+  <si>
+    <t>F-5E</t>
+  </si>
+  <si>
+    <t>A-6A</t>
+  </si>
+  <si>
+    <t>F-14A</t>
+  </si>
+  <si>
+    <t>F-111A</t>
+  </si>
+  <si>
+    <t>F-117</t>
+  </si>
+  <si>
+    <t>F-18A</t>
+  </si>
+  <si>
+    <t>F-105D</t>
+  </si>
+  <si>
+    <t>F-104G</t>
+  </si>
+  <si>
+    <t>T-45A</t>
+  </si>
+  <si>
+    <t>F-8E</t>
+  </si>
+  <si>
+    <t>F-11F</t>
+  </si>
+  <si>
+    <t>Airplance</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Cgrd</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +220,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,17 +256,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1531,6 +1749,937 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Aircraft_main_affect!$U$8:$U$15</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>14634.824405920859</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20445.194503503928</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26263.458695425721</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31972.668817634072</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37917.566427992781</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43694.685748810334</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49490.478708024733</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32750.8898766979</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-601E-4EB3-8DC1-7995E2D8263C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="443073032"/>
+        <c:axId val="443073688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="443073032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="443073688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="443073688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="443073032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Historial data</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Cgrd versus Aspect Ratio</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.10852478997825982"/>
+                  <c:y val="-8.251578761471522E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>maxCl_aspect_ratio!$D$5:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.95</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.77</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.83</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>maxCl_aspect_ratio!$E$5:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.62</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.35</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.36</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.62</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.05</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4D31-4496-8C97-A4DEC0790DA7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="804020792"/>
+        <c:axId val="804019152"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="804020792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Aspect Ratio[-]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="804019152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="804019152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cgrd[-]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="804020792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1611,6 +2760,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2624,6 +3853,1025 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2712,6 +4960,88 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>586155</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>16851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>87924</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>93051</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11F9A3B4-3F0C-4595-B0BB-E28246A7AA66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>227135</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>158993</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>243253</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>73268</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8FAB38E-D22C-49C0-8E9A-C74B117518B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2985,7 +5315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:AG24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -3943,4 +6273,1649 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAD7F8E-9904-4A47-A25B-6DE82CC823BB}">
+  <dimension ref="A2:U36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>68</v>
+      </c>
+      <c r="D4" s="5">
+        <v>18588.1109913285</v>
+      </c>
+      <c r="E4" s="5">
+        <v>6835.0827984969601</v>
+      </c>
+      <c r="F4" s="5">
+        <v>437.42033763865101</v>
+      </c>
+      <c r="G4" s="5">
+        <f>D4-D$36</f>
+        <v>-12423.800921337701</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" ref="H4:I4" si="0">E4-E$36</f>
+        <v>-1257.1139049884496</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" si="0"/>
+        <v>34.582639305531018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>80.8</v>
+      </c>
+      <c r="D5" s="5">
+        <v>22205.2685716796</v>
+      </c>
+      <c r="E5" s="5">
+        <v>7445.9481006911701</v>
+      </c>
+      <c r="F5" s="5">
+        <v>426.12168196124998</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" ref="G5:G35" si="1">D5-D$36</f>
+        <v>-8806.6433409866004</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" ref="H5:H35" si="2">E5-E$36</f>
+        <v>-646.24860279423956</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" ref="I5:I35" si="3">F5-F$36</f>
+        <v>23.283983628129988</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>93.6</v>
+      </c>
+      <c r="D6" s="5">
+        <v>27000.810240888299</v>
+      </c>
+      <c r="E6" s="5">
+        <v>7153.35333228115</v>
+      </c>
+      <c r="F6" s="5">
+        <v>419.46286466699701</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="1"/>
+        <v>-4011.1016717779021</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" si="2"/>
+        <v>-938.84337120425971</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" si="3"/>
+        <v>16.625166333877019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>106.4</v>
+      </c>
+      <c r="D7" s="5">
+        <v>31557.449232259201</v>
+      </c>
+      <c r="E7" s="5">
+        <v>7229.6240369317202</v>
+      </c>
+      <c r="F7" s="5">
+        <v>412.47390999902899</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="1"/>
+        <v>545.53731959300057</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="2"/>
+        <v>-862.57266655368949</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="3"/>
+        <v>9.636211665909002</v>
+      </c>
+      <c r="N7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R7" t="s">
+        <v>16</v>
+      </c>
+      <c r="S7" t="s">
+        <v>17</v>
+      </c>
+      <c r="T7" t="s">
+        <v>18</v>
+      </c>
+      <c r="U7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>119.2</v>
+      </c>
+      <c r="D8" s="5">
+        <v>34873.3518113092</v>
+      </c>
+      <c r="E8" s="5">
+        <v>8275.5590851110192</v>
+      </c>
+      <c r="F8" s="5">
+        <v>400.96574632543201</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="1"/>
+        <v>3861.4398986429987</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="2"/>
+        <v>183.36238162560949</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.8719520076879803</v>
+      </c>
+      <c r="N8">
+        <v>106.4</v>
+      </c>
+      <c r="O8">
+        <v>0.35</v>
+      </c>
+      <c r="P8">
+        <v>10.1</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>40000</v>
+      </c>
+      <c r="S8" s="2">
+        <v>16821.3149115827</v>
+      </c>
+      <c r="T8">
+        <v>2186.49050566184</v>
+      </c>
+      <c r="U8" s="2">
+        <f>S8-T8</f>
+        <v>14634.824405920859</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>132</v>
+      </c>
+      <c r="D9" s="5">
+        <v>35822.049925149302</v>
+      </c>
+      <c r="E9" s="5">
+        <v>9692.7830048358992</v>
+      </c>
+      <c r="F9" s="5">
+        <v>369.85890225289199</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="1"/>
+        <v>4810.1380124831012</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="2"/>
+        <v>1600.5863013504895</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="3"/>
+        <v>-32.978796080227994</v>
+      </c>
+      <c r="N9">
+        <v>106.4</v>
+      </c>
+      <c r="O9">
+        <v>0.4</v>
+      </c>
+      <c r="P9">
+        <v>10.1</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>55000</v>
+      </c>
+      <c r="S9" s="2">
+        <v>23539.961543599598</v>
+      </c>
+      <c r="T9">
+        <v>3094.7670400956699</v>
+      </c>
+      <c r="U9" s="2">
+        <f t="shared" ref="U9:U15" si="4">S9-T9</f>
+        <v>20445.194503503928</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>22995.773642071399</v>
+      </c>
+      <c r="E10" s="3">
+        <v>7008.0017645477801</v>
+      </c>
+      <c r="F10" s="2">
+        <v>195.239530072094</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>-8016.1382705948017</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="2"/>
+        <v>-1084.1949389376296</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="3"/>
+        <v>-207.59816826102599</v>
+      </c>
+      <c r="N10">
+        <v>119.2</v>
+      </c>
+      <c r="O10">
+        <v>0.4</v>
+      </c>
+      <c r="P10">
+        <v>10.1</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>70000</v>
+      </c>
+      <c r="S10" s="2">
+        <v>30321.574447585601</v>
+      </c>
+      <c r="T10">
+        <v>4058.1157521598798</v>
+      </c>
+      <c r="U10" s="2">
+        <f t="shared" si="4"/>
+        <v>26263.458695425721</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="2">
+        <v>28421.769119934601</v>
+      </c>
+      <c r="E11" s="3">
+        <v>7617.1473269257604</v>
+      </c>
+      <c r="F11" s="2">
+        <v>320.81207252303102</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>-2590.1427927315999</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="2"/>
+        <v>-475.04937655964932</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="3"/>
+        <v>-82.025625810088968</v>
+      </c>
+      <c r="N11">
+        <v>119.2</v>
+      </c>
+      <c r="O11">
+        <v>0.4</v>
+      </c>
+      <c r="P11">
+        <v>10.1</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>85000</v>
+      </c>
+      <c r="S11" s="2">
+        <v>37094.804373708503</v>
+      </c>
+      <c r="T11">
+        <v>5122.1355560744296</v>
+      </c>
+      <c r="U11" s="2">
+        <f t="shared" si="4"/>
+        <v>31972.668817634072</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>0.3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>30616.228025275501</v>
+      </c>
+      <c r="E12" s="3">
+        <v>7710.6009849983702</v>
+      </c>
+      <c r="F12" s="2">
+        <v>392.15586756901899</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
+        <v>-395.68388739069997</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="2"/>
+        <v>-381.59571848703945</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="3"/>
+        <v>-10.681830764100994</v>
+      </c>
+      <c r="N12">
+        <v>132</v>
+      </c>
+      <c r="O12">
+        <v>0.4</v>
+      </c>
+      <c r="P12">
+        <v>10.1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>100000</v>
+      </c>
+      <c r="S12" s="2">
+        <v>44023.783213996401</v>
+      </c>
+      <c r="T12">
+        <v>6106.2167860036197</v>
+      </c>
+      <c r="U12" s="2">
+        <f t="shared" si="4"/>
+        <v>37917.566427992781</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>0.35</v>
+      </c>
+      <c r="D13" s="2">
+        <v>31907.3474043854</v>
+      </c>
+      <c r="E13" s="3">
+        <v>8177.0566584032304</v>
+      </c>
+      <c r="F13" s="2">
+        <v>437.85288825082603</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>895.43549171919949</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="2"/>
+        <v>84.859954917820687</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="3"/>
+        <v>35.015189917706039</v>
+      </c>
+      <c r="N13">
+        <v>132</v>
+      </c>
+      <c r="O13">
+        <v>0.4</v>
+      </c>
+      <c r="P13">
+        <v>10.1</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>115000</v>
+      </c>
+      <c r="S13" s="2">
+        <v>50901.045128218997</v>
+      </c>
+      <c r="T13">
+        <v>7206.3593794086601</v>
+      </c>
+      <c r="U13" s="2">
+        <f t="shared" si="4"/>
+        <v>43694.685748810334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>0.4</v>
+      </c>
+      <c r="D14" s="2">
+        <v>32788.501820485399</v>
+      </c>
+      <c r="E14" s="3">
+        <v>8429.8039081362804</v>
+      </c>
+      <c r="F14" s="2">
+        <v>454.38117186007798</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>1776.5899078191978</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="2"/>
+        <v>337.6072046508707</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="3"/>
+        <v>51.543473526957996</v>
+      </c>
+      <c r="N14">
+        <v>132</v>
+      </c>
+      <c r="O14">
+        <v>0.4</v>
+      </c>
+      <c r="P14">
+        <v>10.1</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>130000</v>
+      </c>
+      <c r="S14" s="2">
+        <v>57815.593808248697</v>
+      </c>
+      <c r="T14">
+        <v>8325.1151002239603</v>
+      </c>
+      <c r="U14" s="2">
+        <f t="shared" si="4"/>
+        <v>49490.478708024733</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>0.45</v>
+      </c>
+      <c r="D15" s="2">
+        <v>33462.242406555197</v>
+      </c>
+      <c r="E15" s="3">
+        <v>8696.5130823774907</v>
+      </c>
+      <c r="F15" s="2">
+        <v>460.11721133855798</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>2450.330493888996</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="2"/>
+        <v>604.31637889208105</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="3"/>
+        <v>57.279513005437991</v>
+      </c>
+      <c r="N15">
+        <v>132</v>
+      </c>
+      <c r="O15">
+        <v>0.4</v>
+      </c>
+      <c r="P15">
+        <v>7.3819999999999997</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>145000</v>
+      </c>
+      <c r="S15" s="2">
+        <v>53487.161156978502</v>
+      </c>
+      <c r="T15">
+        <v>20736.271280280602</v>
+      </c>
+      <c r="U15" s="2">
+        <f t="shared" si="4"/>
+        <v>32750.8898766979</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="4">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4">
+        <v>5.57</v>
+      </c>
+      <c r="D16" s="5">
+        <v>30594.37234645</v>
+      </c>
+      <c r="E16" s="5">
+        <v>9381.8327832865798</v>
+      </c>
+      <c r="F16" s="5">
+        <v>362.79344907584698</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="1"/>
+        <v>-417.53956621620091</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" si="2"/>
+        <v>1289.6360798011701</v>
+      </c>
+      <c r="I16" s="5">
+        <f t="shared" si="3"/>
+        <v>-40.044249257273009</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4">
+        <v>6.476</v>
+      </c>
+      <c r="D17" s="5">
+        <v>31877.859036407499</v>
+      </c>
+      <c r="E17" s="5">
+        <v>8856.7900146081902</v>
+      </c>
+      <c r="F17" s="5">
+        <v>395.90366106199502</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="1"/>
+        <v>865.94712374129813</v>
+      </c>
+      <c r="H17" s="5">
+        <f t="shared" si="2"/>
+        <v>764.59331112278051</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" si="3"/>
+        <v>-6.9340372711249643</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4">
+        <v>3</v>
+      </c>
+      <c r="C18" s="4">
+        <v>7.3819999999999997</v>
+      </c>
+      <c r="D18" s="5">
+        <v>32119.785280546701</v>
+      </c>
+      <c r="E18" s="5">
+        <v>8167.0862090504597</v>
+      </c>
+      <c r="F18" s="5">
+        <v>408.62743702037699</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="1"/>
+        <v>1107.8733678805002</v>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" si="2"/>
+        <v>74.889505565050058</v>
+      </c>
+      <c r="I18" s="5">
+        <f t="shared" si="3"/>
+        <v>5.7897386872569996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4">
+        <v>8.2880000000000003</v>
+      </c>
+      <c r="D19" s="5">
+        <v>31369.767517267901</v>
+      </c>
+      <c r="E19" s="5">
+        <v>7515.1376846384101</v>
+      </c>
+      <c r="F19" s="5">
+        <v>416.12761807001698</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="1"/>
+        <v>357.85560460170018</v>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" si="2"/>
+        <v>-577.05901884699961</v>
+      </c>
+      <c r="I19" s="5">
+        <f t="shared" si="3"/>
+        <v>13.289919736896991</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4">
+        <v>3</v>
+      </c>
+      <c r="C20" s="4">
+        <v>9.1940000000000008</v>
+      </c>
+      <c r="D20" s="5">
+        <v>30365.7758290778</v>
+      </c>
+      <c r="E20" s="5">
+        <v>7065.9130156584197</v>
+      </c>
+      <c r="F20" s="5">
+        <v>420.16617126128699</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="1"/>
+        <v>-646.13608358840065</v>
+      </c>
+      <c r="H20" s="5">
+        <f t="shared" si="2"/>
+        <v>-1026.28368782699</v>
+      </c>
+      <c r="I20" s="5">
+        <f t="shared" si="3"/>
+        <v>17.328472928167002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4">
+        <v>10.1</v>
+      </c>
+      <c r="D21" s="5">
+        <v>29250.7053519451</v>
+      </c>
+      <c r="E21" s="5">
+        <v>7043.60847176472</v>
+      </c>
+      <c r="F21" s="5">
+        <v>423.48620280720797</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="1"/>
+        <v>-1761.2065607211007</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="2"/>
+        <v>-1048.5882317206897</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" si="3"/>
+        <v>20.648504474087986</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>31354.762990535899</v>
+      </c>
+      <c r="E22" s="3">
+        <v>8147.7975294703701</v>
+      </c>
+      <c r="F22" s="2">
+        <v>400.74433711661197</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>342.8510778696982</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="2"/>
+        <v>55.600825984960466</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="3"/>
+        <v>-2.0933612165080149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>8.3333333333333304</v>
+      </c>
+      <c r="D23" s="2">
+        <v>31269.9716118621</v>
+      </c>
+      <c r="E23" s="3">
+        <v>8118.4450709291104</v>
+      </c>
+      <c r="F23" s="2">
+        <v>401.642987379923</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>258.05969919589916</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="2"/>
+        <v>26.248367443700772</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="3"/>
+        <v>-1.1947109531969886</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>16.6666666666667</v>
+      </c>
+      <c r="D24" s="2">
+        <v>30914.298918551802</v>
+      </c>
+      <c r="E24" s="3">
+        <v>8102.5532712783897</v>
+      </c>
+      <c r="F24" s="2">
+        <v>402.88267771022498</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="1"/>
+        <v>-97.612994114399044</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="2"/>
+        <v>10.356567792980059</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="3"/>
+        <v>4.4979377104994001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+      <c r="D25" s="2">
+        <v>30468.0826554866</v>
+      </c>
+      <c r="E25" s="3">
+        <v>7993.38344895312</v>
+      </c>
+      <c r="F25" s="2">
+        <v>406.32524910131298</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="1"/>
+        <v>-543.82925717960097</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="2"/>
+        <v>-98.813254532289648</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="3"/>
+        <v>3.4875507681929889</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="4">
+        <v>5</v>
+      </c>
+      <c r="C26" s="4">
+        <v>40000</v>
+      </c>
+      <c r="D26" s="5">
+        <v>14759.491168745801</v>
+      </c>
+      <c r="E26" s="5">
+        <v>4248.3142484987502</v>
+      </c>
+      <c r="F26" s="5">
+        <v>114.85738921551901</v>
+      </c>
+      <c r="G26" s="5">
+        <f t="shared" si="1"/>
+        <v>-16252.4207439204</v>
+      </c>
+      <c r="H26" s="5">
+        <f t="shared" si="2"/>
+        <v>-3843.8824549866595</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" si="3"/>
+        <v>-287.980309117601</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4">
+        <v>5</v>
+      </c>
+      <c r="C27" s="4">
+        <v>55000</v>
+      </c>
+      <c r="D27" s="5">
+        <v>20786.1678825077</v>
+      </c>
+      <c r="E27" s="5">
+        <v>5848.56070118761</v>
+      </c>
+      <c r="F27" s="5">
+        <v>206.128800313243</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="1"/>
+        <v>-10225.744030158501</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" si="2"/>
+        <v>-2243.6360022977997</v>
+      </c>
+      <c r="I27" s="5">
+        <f t="shared" si="3"/>
+        <v>-196.70889801987698</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4">
+        <v>5</v>
+      </c>
+      <c r="C28" s="4">
+        <v>70000</v>
+      </c>
+      <c r="D28" s="5">
+        <v>26939.7612730277</v>
+      </c>
+      <c r="E28" s="5">
+        <v>7439.9289267178701</v>
+      </c>
+      <c r="F28" s="5">
+        <v>321.44342996255801</v>
+      </c>
+      <c r="G28" s="5">
+        <f t="shared" si="1"/>
+        <v>-4072.1506396385012</v>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" si="2"/>
+        <v>-652.26777676753954</v>
+      </c>
+      <c r="I28" s="5">
+        <f t="shared" si="3"/>
+        <v>-81.394268370561974</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4">
+        <v>5</v>
+      </c>
+      <c r="C29" s="4">
+        <v>85000</v>
+      </c>
+      <c r="D29" s="5">
+        <v>33156.177189833099</v>
+      </c>
+      <c r="E29" s="5">
+        <v>9060.7627399498506</v>
+      </c>
+      <c r="F29" s="5">
+        <v>446.83860444724797</v>
+      </c>
+      <c r="G29" s="5">
+        <f t="shared" si="1"/>
+        <v>2144.2652771668982</v>
+      </c>
+      <c r="H29" s="5">
+        <f t="shared" si="2"/>
+        <v>968.56603646444091</v>
+      </c>
+      <c r="I29" s="5">
+        <f t="shared" si="3"/>
+        <v>44.000906114127986</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4">
+        <v>5</v>
+      </c>
+      <c r="C30" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D30" s="5">
+        <v>39591.200827525099</v>
+      </c>
+      <c r="E30" s="5">
+        <v>10538.799172474901</v>
+      </c>
+      <c r="F30" s="5">
+        <v>583.80651066269297</v>
+      </c>
+      <c r="G30" s="5">
+        <f t="shared" si="1"/>
+        <v>8579.2889148588984</v>
+      </c>
+      <c r="H30" s="5">
+        <f t="shared" si="2"/>
+        <v>2446.6024689894912</v>
+      </c>
+      <c r="I30" s="5">
+        <f t="shared" si="3"/>
+        <v>180.96881232957298</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4">
+        <v>5</v>
+      </c>
+      <c r="C31" s="4">
+        <v>115000</v>
+      </c>
+      <c r="D31" s="5">
+        <v>46578.987549062098</v>
+      </c>
+      <c r="E31" s="5">
+        <v>11528.4169585656</v>
+      </c>
+      <c r="F31" s="5">
+        <v>708.97386502058805</v>
+      </c>
+      <c r="G31" s="5">
+        <f t="shared" si="1"/>
+        <v>15567.075636395897</v>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" si="2"/>
+        <v>3436.2202550801903</v>
+      </c>
+      <c r="I31" s="5">
+        <f t="shared" si="3"/>
+        <v>306.13616668746806</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4">
+        <v>5</v>
+      </c>
+      <c r="C32" s="4">
+        <v>130000</v>
+      </c>
+      <c r="D32" s="5">
+        <v>53161.919722686798</v>
+      </c>
+      <c r="E32" s="5">
+        <v>12978.789185785899</v>
+      </c>
+      <c r="F32" s="5">
+        <v>808.05763874368301</v>
+      </c>
+      <c r="G32" s="5">
+        <f t="shared" si="1"/>
+        <v>22150.007810020597</v>
+      </c>
+      <c r="H32" s="5">
+        <f t="shared" si="2"/>
+        <v>4886.5924823004898</v>
+      </c>
+      <c r="I32" s="5">
+        <f t="shared" si="3"/>
+        <v>405.21994041056303</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4">
+        <v>5</v>
+      </c>
+      <c r="C33" s="4">
+        <v>145000</v>
+      </c>
+      <c r="D33" s="5">
+        <v>60317.197526874901</v>
+      </c>
+      <c r="E33" s="5">
+        <v>13906.234910384201</v>
+      </c>
+      <c r="F33" s="5">
+        <v>900.59463688574999</v>
+      </c>
+      <c r="G33" s="5">
+        <f t="shared" si="1"/>
+        <v>29305.2856142087</v>
+      </c>
+      <c r="H33" s="5">
+        <f t="shared" si="2"/>
+        <v>5814.038206898791</v>
+      </c>
+      <c r="I33" s="5">
+        <f t="shared" si="3"/>
+        <v>497.75693855263</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4">
+        <v>5</v>
+      </c>
+      <c r="C34" s="4">
+        <v>160000</v>
+      </c>
+      <c r="D34" s="4">
+        <v>71615.647024054997</v>
+      </c>
+      <c r="E34" s="5">
+        <v>10734.796313901599</v>
+      </c>
+      <c r="F34" s="5">
+        <v>984.40367444675098</v>
+      </c>
+      <c r="G34" s="5">
+        <f t="shared" si="1"/>
+        <v>40603.7351113888</v>
+      </c>
+      <c r="H34" s="5">
+        <f t="shared" si="2"/>
+        <v>2642.5996104161895</v>
+      </c>
+      <c r="I34" s="5">
+        <f t="shared" si="3"/>
+        <v>581.565976113631</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4">
+        <v>5</v>
+      </c>
+      <c r="C35" s="4">
+        <v>175000</v>
+      </c>
+      <c r="D35" s="4">
+        <v>78517.770933178501</v>
+      </c>
+      <c r="E35" s="5">
+        <v>11999.8058657401</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1045.3968675864801</v>
+      </c>
+      <c r="G35" s="5">
+        <f t="shared" si="1"/>
+        <v>47505.859020512304</v>
+      </c>
+      <c r="H35" s="5">
+        <f t="shared" si="2"/>
+        <v>3907.6091622546901</v>
+      </c>
+      <c r="I35" s="5">
+        <f t="shared" si="3"/>
+        <v>642.5591692533601</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>31011.911912666201</v>
+      </c>
+      <c r="E36">
+        <v>8092.1967034854097</v>
+      </c>
+      <c r="F36" s="2">
+        <v>402.83769833311999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB3B4F9-649F-4B57-BCFD-40A46E2E7B01}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36098A4-7930-4260-A0E0-F7ADEE63E561}">
+  <dimension ref="C4:J37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5">
+        <v>1.65</v>
+      </c>
+      <c r="E5">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="E6">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7">
+        <v>3.5</v>
+      </c>
+      <c r="E7">
+        <v>1.2</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8">
+        <v>3.18</v>
+      </c>
+      <c r="E8">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>2.78</v>
+      </c>
+      <c r="E9">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10">
+        <v>3.7</v>
+      </c>
+      <c r="E10">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11">
+        <v>2.9</v>
+      </c>
+      <c r="E11">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>2.36</v>
+      </c>
+      <c r="E12">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13">
+        <v>3.5</v>
+      </c>
+      <c r="E13">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <v>3.2</v>
+      </c>
+      <c r="E14">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15">
+        <v>3.95</v>
+      </c>
+      <c r="E15">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16">
+        <v>6.75</v>
+      </c>
+      <c r="E16">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>5.3</v>
+      </c>
+      <c r="E20">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22">
+        <v>7.25</v>
+      </c>
+      <c r="E22">
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23">
+        <v>7.8</v>
+      </c>
+      <c r="E23">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <v>7.7</v>
+      </c>
+      <c r="E25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26">
+        <v>7.1</v>
+      </c>
+      <c r="E26">
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28">
+        <v>6.95</v>
+      </c>
+      <c r="E28">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <v>7.9</v>
+      </c>
+      <c r="E29">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30">
+        <v>7.77</v>
+      </c>
+      <c r="E30">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E31">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <v>8.5</v>
+      </c>
+      <c r="E32">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33">
+        <v>8.83</v>
+      </c>
+      <c r="E33">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34">
+        <v>9.5</v>
+      </c>
+      <c r="E34">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J37" s="6"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C5:E34">
+    <sortCondition ref="E5:E34"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add benchmarkt case calculation
</commit_message>
<xml_diff>
--- a/Data_analysis.xlsx
+++ b/Data_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keran\Google Drive\MIT\Courses@MIT\Thesis\simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2588C7-DD84-4131-B390-2BD92455BE90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B3A75E-0DBA-42D0-A0D7-2BFC7F022D1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="3975" windowWidth="15480" windowHeight="11010" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15495" yWindow="3315" windowWidth="15480" windowHeight="12000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ship" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Refueling_aircraft" sheetId="3" r:id="rId3"/>
     <sheet name="maxCl_aspect_ratio" sheetId="4" r:id="rId4"/>
     <sheet name="Stakeholder and needs" sheetId="5" r:id="rId5"/>
+    <sheet name="Branchmark Airplane" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
   <si>
     <t>ship length</t>
   </si>
@@ -224,6 +224,91 @@
   </si>
   <si>
     <t>Problem</t>
+  </si>
+  <si>
+    <t>S-3 Viking</t>
+  </si>
+  <si>
+    <t>Boeing 737-200</t>
+  </si>
+  <si>
+    <t>KC-135</t>
+  </si>
+  <si>
+    <t>KC-46</t>
+  </si>
+  <si>
+    <t>Power plant</t>
+  </si>
+  <si>
+    <t>Thr to weight ratio</t>
+  </si>
+  <si>
+    <t>Wing-span[ft]</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>kc135a</t>
+  </si>
+  <si>
+    <t>root: NACA 0016.3-1.03 32.7/100 mod
+tip:NACA 0012-1.10 40/1.00mod</t>
+  </si>
+  <si>
+    <t>root: NACA 64A318;
+tio: NACA 64A412</t>
+  </si>
+  <si>
+    <t>root: BAC 449/450/451;
+tip:BAC442</t>
+  </si>
+  <si>
+    <t>Airfoil[-]</t>
+  </si>
+  <si>
+    <t>Aspect ratio[-]</t>
+  </si>
+  <si>
+    <t>A330-300</t>
+  </si>
+  <si>
+    <t>Max takeoff weight[lb]</t>
+  </si>
+  <si>
+    <t>2x GE TF34-GE-2 turbofan engines</t>
+  </si>
+  <si>
+    <t>4x Allison T56-A-15 turboprop engines</t>
+  </si>
+  <si>
+    <t>PW JT8D-7/9/5/17</t>
+  </si>
+  <si>
+    <t>CFM-56 turbofan engines</t>
+  </si>
+  <si>
+    <t>2 × PW4062</t>
+  </si>
+  <si>
+    <t>2x PW4170</t>
+  </si>
+  <si>
+    <t>Thrusters[lb]</t>
+  </si>
+  <si>
+    <t>C-130J Hercules</t>
+  </si>
+  <si>
+    <t>Operation Empty Weight [lb]</t>
+  </si>
+  <si>
+    <t>Fuel saved
+( 1refueling, 1 airplane)</t>
+  </si>
+  <si>
+    <t>Sweep angle [deg]</t>
   </si>
 </sst>
 </file>
@@ -269,7 +354,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -292,13 +377,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -308,6 +419,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6300,8 +6418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAD7F8E-9904-4A47-A25B-6DE82CC823BB}">
   <dimension ref="A2:U36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView topLeftCell="B22" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7565,7 +7683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB3B4F9-649F-4B57-BCFD-40A46E2E7B01}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
@@ -7945,7 +8063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CB3B78-3196-4725-9489-9F172DB344B8}">
   <dimension ref="G7:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7:J18"/>
     </sheetView>
   </sheetViews>
@@ -7994,4 +8112,280 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA2C042-8FDE-4CB5-8CD4-C64F7A870012}">
+  <dimension ref="B6:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="7">
+        <v>68</v>
+      </c>
+      <c r="D7" s="7">
+        <v>132.6</v>
+      </c>
+      <c r="E7" s="7">
+        <v>93</v>
+      </c>
+      <c r="F7" s="7">
+        <v>130</v>
+      </c>
+      <c r="G7" s="7">
+        <v>157</v>
+      </c>
+      <c r="H7" s="7">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="7">
+        <v>7.73</v>
+      </c>
+      <c r="D9" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="F9" s="7">
+        <v>7.1</v>
+      </c>
+      <c r="G9" s="7">
+        <v>8</v>
+      </c>
+      <c r="H9" s="7">
+        <v>9.26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B10" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="9">
+        <v>26581</v>
+      </c>
+      <c r="D10" s="9">
+        <v>75562</v>
+      </c>
+      <c r="E10" s="9">
+        <v>93680</v>
+      </c>
+      <c r="F10" s="9">
+        <v>105476</v>
+      </c>
+      <c r="G10" s="9">
+        <v>204000</v>
+      </c>
+      <c r="H10" s="9">
+        <v>285300</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B11" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="9">
+        <v>52539</v>
+      </c>
+      <c r="D11" s="9">
+        <v>155000</v>
+      </c>
+      <c r="E11" s="9">
+        <v>181200</v>
+      </c>
+      <c r="F11" s="9">
+        <v>322500</v>
+      </c>
+      <c r="G11" s="9">
+        <v>415000</v>
+      </c>
+      <c r="H11" s="9">
+        <v>533519</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>25</v>
+      </c>
+      <c r="F12" s="11">
+        <v>35</v>
+      </c>
+      <c r="G12" s="11">
+        <v>34</v>
+      </c>
+      <c r="H12" s="11">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B13" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B14" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="7">
+        <f>9275*2</f>
+        <v>18550</v>
+      </c>
+      <c r="D14" s="7">
+        <f>4*7412</f>
+        <v>29648</v>
+      </c>
+      <c r="E14" s="7">
+        <f>29317*2</f>
+        <v>58634</v>
+      </c>
+      <c r="F14" s="7">
+        <f>21600*4</f>
+        <v>86400</v>
+      </c>
+      <c r="G14" s="7">
+        <f>62000*2</f>
+        <v>124000</v>
+      </c>
+      <c r="H14" s="7">
+        <f>72000*2</f>
+        <v>144000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="10">
+        <f t="shared" ref="C15:G15" si="0">C14/C11</f>
+        <v>0.35307105198043359</v>
+      </c>
+      <c r="D15" s="10">
+        <f t="shared" si="0"/>
+        <v>0.19127741935483872</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="0"/>
+        <v>0.32358719646799117</v>
+      </c>
+      <c r="F15" s="7">
+        <f t="shared" si="0"/>
+        <v>0.26790697674418606</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="0"/>
+        <v>0.29879518072289157</v>
+      </c>
+      <c r="H15" s="7">
+        <f>H14/H11</f>
+        <v>0.269906038960187</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B16" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
import the climb simulation due to the nonlinearity
</commit_message>
<xml_diff>
--- a/Data_analysis.xlsx
+++ b/Data_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keran\Google Drive\MIT\Courses@MIT\Thesis\simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B3A75E-0DBA-42D0-A0D7-2BFC7F022D1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15B7CBC-4F41-46BF-944D-B3CB24322EF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15495" yWindow="3315" windowWidth="15480" windowHeight="12000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ship" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
   <si>
     <t>ship length</t>
   </si>
@@ -304,11 +304,22 @@
     <t>Operation Empty Weight [lb]</t>
   </si>
   <si>
-    <t>Fuel saved
-( 1refueling, 1 airplane)</t>
-  </si>
-  <si>
     <t>Sweep angle [deg]</t>
+  </si>
+  <si>
+    <t>Take-off distance[ft]
+(Simulations)</t>
+  </si>
+  <si>
+    <t>Take-off distance[ft]
+(From reference)</t>
+  </si>
+  <si>
+    <t>Fuel saved[lb]
+(capacity - fuel cost)</t>
+  </si>
+  <si>
+    <t>Aircraft type</t>
   </si>
 </sst>
 </file>
@@ -354,7 +365,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -392,24 +403,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -425,7 +425,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -8116,25 +8118,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA2C042-8FDE-4CB5-8CD4-C64F7A870012}">
-  <dimension ref="B6:H16"/>
+  <dimension ref="B6:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.53125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="C6" s="7" t="s">
         <v>62</v>
       </c>
@@ -8270,25 +8273,25 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="7">
         <v>15</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="7">
         <v>0</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="7">
         <v>25</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="12">
         <v>35</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="12">
         <v>34</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="12">
         <v>29.7</v>
       </c>
     </row>
@@ -8373,16 +8376,155 @@
         <v>0.269906038960187</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B16" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+        <v>90</v>
+      </c>
+      <c r="C16" s="7">
+        <v>19290.152768622502</v>
+      </c>
+      <c r="D16" s="7">
+        <v>57370.141780962404</v>
+      </c>
+      <c r="E16" s="7">
+        <v>76090.287190284595</v>
+      </c>
+      <c r="F16" s="7">
+        <v>84178.868950823904</v>
+      </c>
+      <c r="G16" s="7">
+        <v>197443.268339662</v>
+      </c>
+      <c r="H16" s="7">
+        <v>236349.10957827399</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B17" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="7">
+        <v>3824.7660513424298</v>
+      </c>
+      <c r="D17" s="7">
+        <v>7658.8496809376602</v>
+      </c>
+      <c r="E17" s="7">
+        <v>9214.4947956890701</v>
+      </c>
+      <c r="F17" s="7">
+        <v>7975.4244536544002</v>
+      </c>
+      <c r="G17" s="7">
+        <v>5831.06606979138</v>
+      </c>
+      <c r="H17" s="7">
+        <v>7212.7503447723002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B18" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="7">
+        <v>4700</v>
+      </c>
+      <c r="E18" s="7">
+        <v>9700</v>
+      </c>
+      <c r="F18" s="7">
+        <v>7000</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="13">
+        <v>7280</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="J20">
+        <v>3824.7660513424298</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="H21" s="1"/>
+      <c r="J21">
+        <v>7658.8496809376602</v>
+      </c>
+      <c r="L21">
+        <v>19290.152768622502</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="J22">
+        <v>9214.4947956890701</v>
+      </c>
+      <c r="L22">
+        <v>57370.141780962404</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="J23">
+        <v>7975.4244536544002</v>
+      </c>
+      <c r="L23" s="11">
+        <v>-1.47499760874821E+16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="J24">
+        <v>5831.06606979138</v>
+      </c>
+      <c r="L24">
+        <v>84178.868950823904</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="J25">
+        <v>7212.7503447723002</v>
+      </c>
+      <c r="L25">
+        <v>197443.268339662</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="L26">
+        <v>236349.10957827399</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="F27">
+        <v>3824.7660513424298</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="F28">
+        <v>7658.8496809376602</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="F29">
+        <v>9214.4947956890701</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="F30">
+        <v>7975.4244536544002</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="F31">
+        <v>5831.06606979138</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="F32">
+        <v>7212.7503447723002</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rerrange the scirpt to be more lean
</commit_message>
<xml_diff>
--- a/Data_analysis.xlsx
+++ b/Data_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keran\Google Drive\MIT\Courses@MIT\Thesis\simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15B7CBC-4F41-46BF-944D-B3CB24322EF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8434D784-BF34-41F7-8474-EE2368C64011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28898" yWindow="-68" windowWidth="28996" windowHeight="15796" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ship" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="maxCl_aspect_ratio" sheetId="4" r:id="rId4"/>
     <sheet name="Stakeholder and needs" sheetId="5" r:id="rId5"/>
     <sheet name="Branchmark Airplane" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="105">
   <si>
     <t>ship length</t>
   </si>
@@ -320,6 +321,46 @@
   </si>
   <si>
     <t>Aircraft type</t>
+  </si>
+  <si>
+    <t>Range(ship)[km]</t>
+  </si>
+  <si>
+    <t>Range(island)[km]</t>
+  </si>
+  <si>
+    <t>Run way limits[ft]</t>
+  </si>
+  <si>
+    <t>Ship runway limits[ft]</t>
+  </si>
+  <si>
+    <t>Optimization using simulated annealing</t>
+  </si>
+  <si>
+    <t>Wing span[ft]</t>
+  </si>
+  <si>
+    <t>thr to weight ratio[-]</t>
+  </si>
+  <si>
+    <t>aspect ratio[-]</t>
+  </si>
+  <si>
+    <t>sweep angle[deg]</t>
+  </si>
+  <si>
+    <t>max takeoff weight[lb]</t>
+  </si>
+  <si>
+    <t>Case #</t>
+  </si>
+  <si>
+    <t>Take-off distance[ft] 1.1 margin
+(Simulations)</t>
+  </si>
+  <si>
+    <t>FUEL SAVED</t>
   </si>
 </sst>
 </file>
@@ -409,7 +450,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -419,15 +460,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -8118,171 +8175,172 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA2C042-8FDE-4CB5-8CD4-C64F7A870012}">
-  <dimension ref="B6:L32"/>
+  <dimension ref="B6:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="23.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.46484375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="15.9296875" customWidth="1"/>
+    <col min="7" max="7" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="9" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="9">
         <v>68</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="9">
         <v>132.6</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="9">
         <v>93</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="9">
         <v>130</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="9">
         <v>157</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="9">
         <v>198</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="9">
         <v>7.73</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="9">
         <v>10.1</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="9">
         <v>9.4499999999999993</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="9">
         <v>7.1</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="9">
         <v>8</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="9">
         <v>9.26</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="11">
         <v>26581</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="11">
         <v>75562</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="11">
         <v>93680</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="11">
         <v>105476</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="11">
         <v>204000</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="11">
         <v>285300</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="11">
         <v>52539</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="11">
         <v>155000</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="11">
         <v>181200</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="11">
         <v>322500</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="11">
         <v>415000</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="11">
         <v>533519</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="9">
         <v>15</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="9">
         <v>0</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="9">
         <v>25</v>
       </c>
       <c r="F12" s="12">
@@ -8296,238 +8354,461 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="9">
         <f>9275*2</f>
         <v>18550</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="9">
         <f>4*7412</f>
         <v>29648</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="9">
         <f>29317*2</f>
         <v>58634</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="9">
         <f>21600*4</f>
         <v>86400</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="9">
         <f>62000*2</f>
         <v>124000</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="9">
         <f>72000*2</f>
         <v>144000</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="13">
         <f t="shared" ref="C15:G15" si="0">C14/C11</f>
         <v>0.35307105198043359</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="13">
         <f t="shared" si="0"/>
         <v>0.19127741935483872</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="9">
         <f t="shared" si="0"/>
         <v>0.32358719646799117</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="9">
         <f t="shared" si="0"/>
         <v>0.26790697674418606</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="9">
         <f t="shared" si="0"/>
         <v>0.29879518072289157</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="9">
         <f>H14/H11</f>
         <v>0.269906038960187</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="7">
-        <v>19290.152768622502</v>
-      </c>
-      <c r="D16" s="7">
-        <v>57370.141780962404</v>
-      </c>
-      <c r="E16" s="7">
-        <v>76090.287190284595</v>
-      </c>
-      <c r="F16" s="7">
-        <v>84178.868950823904</v>
-      </c>
-      <c r="G16" s="7">
-        <v>197443.268339662</v>
-      </c>
-      <c r="H16" s="7">
-        <v>236349.10957827399</v>
+      <c r="C16" s="11">
+        <v>16353.2425826376</v>
+      </c>
+      <c r="D16" s="11">
+        <v>49214.444181069703</v>
+      </c>
+      <c r="E16" s="11">
+        <v>66160.043385847996</v>
+      </c>
+      <c r="F16" s="11">
+        <v>73861.227986158905</v>
+      </c>
+      <c r="G16" s="11">
+        <v>173694.952401569</v>
+      </c>
+      <c r="H16" s="11">
+        <v>206932.244301542</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="9">
         <v>3824.7660513424298</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="9">
         <v>7658.8496809376602</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="9">
         <v>9214.4947956890701</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="9">
         <v>7975.4244536544002</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="9">
         <v>5831.06606979138</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="9">
         <v>7212.7503447723002</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="9">
         <v>4700</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="9">
         <v>9700</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="9">
         <v>7000</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="14">
         <v>7280</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="J20">
-        <v>3824.7660513424298</v>
+    <row r="20" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B20" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20">
+        <v>3433.5367253872801</v>
+      </c>
+      <c r="D20">
+        <v>7762.6418483978396</v>
+      </c>
+      <c r="E20">
+        <v>8659.8757447735898</v>
+      </c>
+      <c r="F20">
+        <v>7626.3734160430404</v>
+      </c>
+      <c r="G20">
+        <v>5679.3101547331999</v>
+      </c>
+      <c r="H20">
+        <v>6704.4421894425705</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.45">
       <c r="H21" s="1"/>
-      <c r="J21">
-        <v>7658.8496809376602</v>
-      </c>
-      <c r="L21">
-        <v>19290.152768622502</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="J22">
-        <v>9214.4947956890701</v>
-      </c>
-      <c r="L22">
-        <v>57370.141780962404</v>
-      </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="J23">
-        <v>7975.4244536544002</v>
-      </c>
-      <c r="L23" s="11">
-        <v>-1.47499760874821E+16</v>
-      </c>
+      <c r="L23" s="8"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="J24">
-        <v>5831.06606979138</v>
-      </c>
-      <c r="L24">
-        <v>84178.868950823904</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="J25">
-        <v>7212.7503447723002</v>
-      </c>
-      <c r="L25">
-        <v>197443.268339662</v>
+      <c r="B24" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="15"/>
+    </row>
+    <row r="25" spans="2:12" s="7" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B25" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="L26">
-        <v>236349.10957827399</v>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>500</v>
+      </c>
+      <c r="D26">
+        <v>900</v>
+      </c>
+      <c r="E26">
+        <v>9000</v>
+      </c>
+      <c r="F26">
+        <v>205</v>
+      </c>
+      <c r="G26">
+        <v>120.96161081621101</v>
+      </c>
+      <c r="H26">
+        <v>0.35</v>
+      </c>
+      <c r="I26">
+        <v>5.57270323280882</v>
+      </c>
+      <c r="J26">
+        <v>23.522281247699901</v>
+      </c>
+      <c r="K26">
+        <v>137324.62388941899</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>500</v>
+      </c>
+      <c r="D27">
+        <v>900</v>
+      </c>
+      <c r="E27">
+        <v>9000</v>
+      </c>
       <c r="F27">
-        <v>3824.7660513424298</v>
+        <v>245</v>
+      </c>
+      <c r="G27">
+        <v>105.556417897317</v>
+      </c>
+      <c r="H27">
+        <v>0.34982551871945899</v>
+      </c>
+      <c r="I27">
+        <v>5.6132254754894104</v>
+      </c>
+      <c r="J27">
+        <v>0.31863630739584903</v>
+      </c>
+      <c r="K27">
+        <v>118574.770218673</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>500</v>
+      </c>
+      <c r="D28">
+        <v>900</v>
+      </c>
+      <c r="E28">
+        <v>9000</v>
+      </c>
       <c r="F28">
-        <v>7658.8496809376602</v>
+        <v>285</v>
+      </c>
+      <c r="G28">
+        <v>127.26848721229</v>
+      </c>
+      <c r="H28">
+        <v>0.35</v>
+      </c>
+      <c r="I28">
+        <v>5.5428819204567104</v>
+      </c>
+      <c r="J28">
+        <v>21.928792935022699</v>
+      </c>
+      <c r="K28">
+        <v>153024.91898027199</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>500</v>
+      </c>
+      <c r="D29">
+        <v>900</v>
+      </c>
+      <c r="E29">
+        <v>9000</v>
+      </c>
       <c r="F29">
-        <v>9214.4947956890701</v>
+        <v>330</v>
+      </c>
+      <c r="G29">
+        <v>131.82494344988299</v>
+      </c>
+      <c r="H29">
+        <v>0.35</v>
+      </c>
+      <c r="I29">
+        <v>5.9679445831296798</v>
+      </c>
+      <c r="J29">
+        <v>24.371864113890702</v>
+      </c>
+      <c r="K29">
+        <v>157925.982587951</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>500</v>
+      </c>
+      <c r="D30">
+        <v>900</v>
+      </c>
+      <c r="E30">
+        <v>9000</v>
+      </c>
       <c r="F30">
-        <v>7975.4244536544002</v>
+        <v>415</v>
+      </c>
+      <c r="G30">
+        <v>128.2603542905</v>
+      </c>
+      <c r="H30">
+        <v>0.35</v>
+      </c>
+      <c r="I30">
+        <v>5.57709068728267</v>
+      </c>
+      <c r="J30">
+        <v>19.585818931124098</v>
+      </c>
+      <c r="K30">
+        <v>169949.95488569399</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>500</v>
+      </c>
+      <c r="D31">
+        <v>900</v>
+      </c>
+      <c r="E31">
+        <v>9000</v>
+      </c>
       <c r="F31">
-        <v>5831.06606979138</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="F32">
-        <v>7212.7503447723002</v>
+        <v>9000</v>
+      </c>
+      <c r="G31">
+        <v>128.2603542905</v>
+      </c>
+      <c r="H31">
+        <v>0.35</v>
+      </c>
+      <c r="I31">
+        <v>10.1</v>
+      </c>
+      <c r="J31">
+        <v>19.585818931124098</v>
+      </c>
+      <c r="K31">
+        <v>169949.95488569399</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D48">
+        <v>7762.6418483978396</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D49">
+        <v>8659.8757447735898</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D50">
+        <v>7626.3734160430404</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D51">
+        <v>5679.3101547331999</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D52">
+        <v>6704.4421894425705</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B24:C24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F11B450-16D2-4789-ABB9-2C8246930002}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>